<commit_message>
finish the marking and things
</commit_message>
<xml_diff>
--- a/MessagePeopleFromExcel/Auckland Bussiness Strategies.xlsx
+++ b/MessagePeopleFromExcel/Auckland Bussiness Strategies.xlsx
@@ -4848,12 +4848,27 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -4874,10 +4889,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5193,7 +5211,7 @@
   <dimension ref="A1:A1605"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5212,67 +5230,67 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>